<commit_message>
modified sample question file
</commit_message>
<xml_diff>
--- a/clintwin/sponsor/static/sponsor/sample_file/sample_trial_questions.xlsx
+++ b/clintwin/sponsor/static/sponsor/sample_file/sample_trial_questions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adaeze/clintwin360/ClinTwin360_Web/clintwin/sponsor/static/sponsor/sample_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C60EA47-A17A-914F-9075-B86DE3413666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD3F9A5-C60A-BE4B-905A-2435D52DD5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_trial_questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Instructions and Parameter" sheetId="2" r:id="rId2"/>
+    <sheet name="Instructions and Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Do you have a healthcare provider?</t>
   </si>
   <si>
-    <t>[\"Single\";\"Married\";\"Widowed\"; \"Divorced\"; \"Separated\"; \"Registered partnership\"]</t>
-  </si>
-  <si>
-    <t>[\"Yes\";\"No\"]</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -93,25 +87,34 @@
     <t>How old are you?</t>
   </si>
   <si>
-    <t>{\"min\":0;\"max\":140;\"increment\":1,\"unit\":\"years\"}</t>
-  </si>
-  <si>
     <t>Instructions</t>
   </si>
   <si>
-    <t>Enter in the questions and the the possible options for answers using the format in the previous sheet</t>
-  </si>
-  <si>
-    <t>Select the correct valueType</t>
-  </si>
-  <si>
     <t>Save as .CSV file and upload to website</t>
+  </si>
+  <si>
+    <t>["Single";"Married";"Widowed"; "Divorced"; "Separated"; "Registered partnership"]</t>
+  </si>
+  <si>
+    <t>["Yes";"No"]</t>
+  </si>
+  <si>
+    <t>{"min":0;"max":140;"increment":1;"unit":"years"}</t>
+  </si>
+  <si>
+    <t>Then select the valueType that best suits the question</t>
+  </si>
+  <si>
+    <t>Enter in the questions</t>
+  </si>
+  <si>
+    <t>Enter possible options for answers using the format in the previous sheet titled, "sample_trial_questions"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -129,14 +132,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -150,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -158,18 +161,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -486,23 +511,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="54.5" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -516,7 +541,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -526,11 +551,11 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -540,161 +565,161 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="C22" t="s">
@@ -702,7 +727,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="C23" t="s">
@@ -710,7 +735,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="C24" t="s">
@@ -718,7 +743,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="C25" t="s">
@@ -726,7 +751,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="C26" t="s">
@@ -734,7 +759,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="C27" t="s">
@@ -742,7 +767,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="C28" t="s">
@@ -750,7 +775,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="C29" t="s">
@@ -758,7 +783,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="C30" t="s">
@@ -766,7 +791,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="C31" t="s">
@@ -778,9 +803,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>'Instructions and Parameter'!$B$3:$B$7</xm:f>
+            <xm:f>'Instructions and Parameters'!$B$3:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C31</xm:sqref>
         </x14:dataValidation>
@@ -791,98 +816,144 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="5" spans="1:3">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="6" spans="1:3">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="7" spans="1:3">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="9">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="9">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>